<commit_message>
Fin bâtiments + tous twy/apron
reste arbres + divers objets
</commit_message>
<xml_diff>
--- a/LFPN_FR.ASG/Correspondance.xlsx
+++ b/LFPN_FR.ASG/Correspondance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>E1</t>
   </si>
@@ -213,21 +213,12 @@
     <t>Tudair / Golf Tango</t>
   </si>
   <si>
-    <t>Aero club Ouest Parisien</t>
-  </si>
-  <si>
-    <t>IX AIR / First Flight</t>
-  </si>
-  <si>
     <t>Essence</t>
   </si>
   <si>
     <t>Aéro Touring Club de France</t>
   </si>
   <si>
-    <t>HélixAero / Clean Aéro Service</t>
-  </si>
-  <si>
     <t>221 - 223</t>
   </si>
   <si>
@@ -292,6 +283,21 @@
   </si>
   <si>
     <t>Alcyons</t>
+  </si>
+  <si>
+    <t>Restaurant Air &amp; Cook</t>
+  </si>
+  <si>
+    <t>Aero club Ouest Parisien - ACOP</t>
+  </si>
+  <si>
+    <t>Clean Aéro Service</t>
+  </si>
+  <si>
+    <t>IX AIR Helix Aero  First Flight</t>
+  </si>
+  <si>
+    <t>JC Decaux</t>
   </si>
 </sst>
 </file>
@@ -629,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +653,7 @@
         <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,7 +664,7 @@
         <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +675,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,7 +686,7 @@
         <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +697,7 @@
         <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +708,7 @@
         <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,10 +716,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +730,7 @@
         <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,10 +738,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +752,7 @@
         <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +763,7 @@
         <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,7 +785,7 @@
         <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,7 +804,7 @@
         <v>121122</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -825,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -836,7 +842,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,7 +853,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,7 +864,7 @@
         <v>201</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +875,7 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,10 +905,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +938,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,6 +948,9 @@
       <c r="B29" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -951,7 +960,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,7 +968,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="1">
-        <v>243</v>
+        <v>245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,7 +982,7 @@
         <v>247</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +1001,7 @@
         <v>403</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1043,7 +1055,7 @@
         <v>309</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>